<commit_message>
Add Reroute script for staging and update data path
</commit_message>
<xml_diff>
--- a/testdata/FCfiles/stg/RequestReroute/QuickQuoteTestData.xlsx
+++ b/testdata/FCfiles/stg/RequestReroute/QuickQuoteTestData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="388">
   <si>
     <t>shipmentType</t>
   </si>
@@ -1155,6 +1155,42 @@
   </si>
   <si>
     <t>FCUPSG1011889</t>
+  </si>
+  <si>
+    <t>58542851</t>
+  </si>
+  <si>
+    <t>01-23-2022</t>
+  </si>
+  <si>
+    <t>$489.35</t>
+  </si>
+  <si>
+    <t>FCBTXA1000044</t>
+  </si>
+  <si>
+    <t>58542852</t>
+  </si>
+  <si>
+    <t>$62.43</t>
+  </si>
+  <si>
+    <t>1Z44R7R60392591163</t>
+  </si>
+  <si>
+    <t>FCUPSG1506810</t>
+  </si>
+  <si>
+    <t>58542853</t>
+  </si>
+  <si>
+    <t>$151.56</t>
+  </si>
+  <si>
+    <t>1Z44R7R60392395189</t>
+  </si>
+  <si>
+    <t>FCUPSG1506811</t>
   </si>
 </sst>
 </file>
@@ -1190,7 +1226,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="564">
+  <fills count="594">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4007,8 +4043,158 @@
         <fgColor indexed="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="560">
+  <borders count="590">
     <border>
       <left/>
       <right/>
@@ -6524,6 +6710,111 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
@@ -6532,7 +6823,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="331">
+  <cellXfs count="346">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
@@ -6863,7 +7154,22 @@
     <xf applyBorder="true" applyFill="true" borderId="553" fillId="557" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="555" fillId="559" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="557" fillId="561" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="563" borderId="559" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf applyBorder="true" applyFill="true" borderId="559" fillId="563" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="561" fillId="565" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="563" fillId="567" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="565" fillId="569" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="567" fillId="571" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="569" fillId="573" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="571" fillId="575" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="573" fillId="577" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="575" fillId="579" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="577" fillId="581" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="579" fillId="583" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="581" fillId="585" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="583" fillId="587" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="585" fillId="589" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="587" fillId="591" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="593" borderId="589" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
@@ -7511,8 +7817,8 @@
       <c r="A2" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="317" t="s">
-        <v>366</v>
+      <c r="B2" s="332" t="s">
+        <v>377</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>18</v>
@@ -7563,20 +7869,20 @@
       <c r="U2" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="V2" s="316" t="s">
-        <v>365</v>
+      <c r="V2" s="331" t="s">
+        <v>376</v>
       </c>
       <c r="W2" s="235" t="s">
         <v>309</v>
       </c>
-      <c r="X2" s="318" t="s">
-        <v>148</v>
-      </c>
-      <c r="Y2" s="319" t="s">
-        <v>367</v>
-      </c>
-      <c r="Z2" s="320" t="s">
-        <v>367</v>
+      <c r="X2" s="333" t="s">
+        <v>378</v>
+      </c>
+      <c r="Y2" s="334" t="s">
+        <v>379</v>
+      </c>
+      <c r="Z2" s="335" t="s">
+        <v>379</v>
       </c>
       <c r="AA2" s="15" t="s">
         <v>147</v>
@@ -8153,8 +8459,8 @@
       <c r="A9" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="322" t="s">
-        <v>366</v>
+      <c r="B9" s="337" t="s">
+        <v>377</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>21</v>
@@ -8205,20 +8511,20 @@
       <c r="U9" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="V9" s="321" t="s">
-        <v>368</v>
+      <c r="V9" s="336" t="s">
+        <v>380</v>
       </c>
       <c r="W9" s="20" t="s">
         <v>153</v>
       </c>
-      <c r="X9" s="323" t="s">
-        <v>369</v>
-      </c>
-      <c r="Y9" s="324" t="s">
-        <v>370</v>
-      </c>
-      <c r="Z9" s="325" t="s">
-        <v>371</v>
+      <c r="X9" s="338" t="s">
+        <v>381</v>
+      </c>
+      <c r="Y9" s="339" t="s">
+        <v>382</v>
+      </c>
+      <c r="Z9" s="340" t="s">
+        <v>383</v>
       </c>
       <c r="AA9" s="14" t="s">
         <v>146</v>
@@ -8321,8 +8627,8 @@
       <c r="A11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="327" t="s">
-        <v>366</v>
+      <c r="B11" s="342" t="s">
+        <v>377</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>21</v>
@@ -8373,20 +8679,20 @@
       <c r="U11" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="V11" s="326" t="s">
-        <v>372</v>
+      <c r="V11" s="341" t="s">
+        <v>384</v>
       </c>
       <c r="W11" s="21" t="s">
         <v>154</v>
       </c>
-      <c r="X11" s="328" t="s">
-        <v>373</v>
-      </c>
-      <c r="Y11" s="329" t="s">
-        <v>374</v>
-      </c>
-      <c r="Z11" s="330" t="s">
-        <v>375</v>
+      <c r="X11" s="343" t="s">
+        <v>385</v>
+      </c>
+      <c r="Y11" s="344" t="s">
+        <v>386</v>
+      </c>
+      <c r="Z11" s="345" t="s">
+        <v>387</v>
       </c>
       <c r="AA11" s="14" t="s">
         <v>146</v>

</xml_diff>